<commit_message>
add result of runtimeverification
</commit_message>
<xml_diff>
--- a/実験結果まとめ.xlsx
+++ b/実験結果まとめ.xlsx
@@ -9,12 +9,13 @@
   </bookViews>
   <sheets>
     <sheet name="結果まとめ" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Detection_Rate比較" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="FPRate比較" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="ファイル名とIDの対応表" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="結果まとめ_新版" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Detection_Rate比較" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="FPRate比較" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="ファイル名とIDの対応表" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">ファイル名とIDの対応表!$B$1:$E$52</definedName>
+    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">ファイル名とIDの対応表!$B$1:$E$52</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="265">
   <si>
     <t xml:space="preserve"># of variations</t>
   </si>
@@ -256,6 +257,44 @@
     <t xml:space="preserve">memory_allocation_failure.c</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">OOM Killer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">に殺されたり、全く意図外の箇所を発見したため、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">とした。</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Memory leakage</t>
   </si>
   <si>
@@ -629,6 +668,9 @@
   </si>
   <si>
     <t xml:space="preserve">double_release.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">旧版での発見率</t>
   </si>
   <si>
     <t xml:space="preserve">Detection Rate</t>
@@ -1302,7 +1344,7 @@
     <xf numFmtId="164" fontId="11" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1391,7 +1433,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1484,7 +1542,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1528,7 +1586,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Detection_Rate比較!$C$1</c:f>
+              <c:f>Detection_Rate比較!$C$1:$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1619,7 +1677,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Detection_Rate比較!$D$1</c:f>
+              <c:f>Detection_Rate比較!$D$1:$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1696,7 +1754,7 @@
                   <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.53125</c:v>
+                  <c:v>0.46875</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.607142857142857</c:v>
@@ -1710,7 +1768,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Detection_Rate比較!$E$1</c:f>
+              <c:f>Detection_Rate比較!$E$1:$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1801,7 +1859,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Detection_Rate比較!$F$1</c:f>
+              <c:f>Detection_Rate比較!$F$1:$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1892,7 +1950,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Detection_Rate比較!$G$1</c:f>
+              <c:f>Detection_Rate比較!$G$1:$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1980,11 +2038,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="98799223"/>
-        <c:axId val="50658142"/>
+        <c:axId val="40202789"/>
+        <c:axId val="38462007"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="98799223"/>
+        <c:axId val="40202789"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2012,14 +2070,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50658142"/>
+        <c:crossAx val="38462007"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50658142"/>
+        <c:axId val="38462007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2057,7 +2115,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98799223"/>
+        <c:crossAx val="40202789"/>
         <c:crossesAt val="1"/>
       </c:valAx>
       <c:spPr>
@@ -2104,7 +2162,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2148,7 +2206,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>FPRate比較!$C$1</c:f>
+              <c:f>FPRate比較!$C$1:$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2239,7 +2297,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>FPRate比較!$D$1</c:f>
+              <c:f>FPRate比較!$D$1:$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2330,7 +2388,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>FPRate比較!$E$1</c:f>
+              <c:f>FPRate比較!$E$1:$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2421,7 +2479,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>FPRate比較!$F$1</c:f>
+              <c:f>FPRate比較!$F$1:$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2509,11 +2567,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="49536875"/>
-        <c:axId val="79760833"/>
+        <c:axId val="47272220"/>
+        <c:axId val="86625541"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="49536875"/>
+        <c:axId val="47272220"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2541,14 +2599,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79760833"/>
+        <c:crossAx val="86625541"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79760833"/>
+        <c:axId val="86625541"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2587,7 +2645,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49536875"/>
+        <c:crossAx val="47272220"/>
         <c:crossesAt val="1"/>
       </c:valAx>
       <c:spPr>
@@ -2715,10 +2773,10 @@
   </sheetPr>
   <dimension ref="A1:R53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="I3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="P6" activeCellId="0" sqref="P6"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3128,63 +3186,65 @@
       <c r="P8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="n">
+      <c r="A9" s="9" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="12" t="n">
+      <c r="D9" s="9" t="n">
         <v>16</v>
       </c>
-      <c r="E9" s="12" t="n">
+      <c r="E9" s="9" t="n">
         <v>16</v>
       </c>
-      <c r="F9" s="12" t="n">
+      <c r="F9" s="9" t="n">
         <v>28</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="12" t="n">
+      <c r="I9" s="9" t="n">
         <f aca="false">J9+K9</f>
-        <v>6</v>
-      </c>
-      <c r="J9" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" s="12" t="n">
-        <v>6</v>
-      </c>
-      <c r="L9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="9" t="n">
         <f aca="false">D9-I9</f>
-        <v>10</v>
-      </c>
-      <c r="M9" s="14" t="n">
+        <v>16</v>
+      </c>
+      <c r="M9" s="11" t="n">
         <f aca="false">I9/D9</f>
-        <v>0.375</v>
-      </c>
-      <c r="N9" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="9" t="n">
         <f aca="false">E9-N9</f>
         <v>16</v>
       </c>
-      <c r="P9" s="12"/>
+      <c r="P9" s="9" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="n">
         <v>8</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>37</v>
@@ -3199,7 +3259,7 @@
         <v>29</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>21</v>
@@ -3230,7 +3290,7 @@
         <v>18</v>
       </c>
       <c r="P10" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3238,7 +3298,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>37</v>
@@ -3253,7 +3313,7 @@
         <v>38</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>21</v>
@@ -3290,7 +3350,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>37</v>
@@ -3305,7 +3365,7 @@
         <v>45</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H12" s="13" t="s">
         <v>21</v>
@@ -3342,7 +3402,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>37</v>
@@ -3357,7 +3417,7 @@
         <v>12</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>21</v>
@@ -3394,7 +3454,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>37</v>
@@ -3409,7 +3469,7 @@
         <v>16</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>21</v>
@@ -3446,10 +3506,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D15" s="6" t="n">
         <v>14</v>
@@ -3461,7 +3521,7 @@
         <v>17</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>21</v>
@@ -3498,10 +3558,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D16" s="12" t="n">
         <v>15</v>
@@ -3513,7 +3573,7 @@
         <v>18</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H16" s="13" t="s">
         <v>21</v>
@@ -3550,10 +3610,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D17" s="6" t="n">
         <v>17</v>
@@ -3565,7 +3625,7 @@
         <v>31</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>21</v>
@@ -3602,10 +3662,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D18" s="9" t="n">
         <v>2</v>
@@ -3617,7 +3677,7 @@
         <v>35</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H18" s="10" t="s">
         <v>21</v>
@@ -3648,7 +3708,7 @@
         <v>2</v>
       </c>
       <c r="P18" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3656,10 +3716,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D19" s="6" t="n">
         <v>16</v>
@@ -3671,7 +3731,7 @@
         <v>46</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>21</v>
@@ -3708,10 +3768,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D20" s="6" t="n">
         <v>18</v>
@@ -3723,7 +3783,7 @@
         <v>50</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>21</v>
@@ -3760,10 +3820,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D21" s="9" t="n">
         <v>2</v>
@@ -3775,7 +3835,7 @@
         <v>4</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H21" s="10" t="s">
         <v>21</v>
@@ -3806,7 +3866,7 @@
         <v>2</v>
       </c>
       <c r="P21" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3814,10 +3874,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D22" s="15" t="n">
         <v>29</v>
@@ -3829,10 +3889,10 @@
         <v>34</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I22" s="17" t="n">
         <v>0</v>
@@ -3856,10 +3916,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D23" s="15" t="n">
         <v>19</v>
@@ -3871,10 +3931,10 @@
         <v>39</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I23" s="17" t="n">
         <v>0</v>
@@ -3898,10 +3958,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D24" s="15" t="n">
         <v>16</v>
@@ -3913,10 +3973,10 @@
         <v>51</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I24" s="17" t="n">
         <v>14</v>
@@ -3935,10 +3995,10 @@
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
       <c r="Q24" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3946,10 +4006,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D25" s="15" t="n">
         <v>17</v>
@@ -3961,10 +4021,10 @@
         <v>1</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I25" s="17" t="n">
         <v>16</v>
@@ -3983,10 +4043,10 @@
       <c r="O25" s="15"/>
       <c r="P25" s="15"/>
       <c r="Q25" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3994,10 +4054,10 @@
         <v>24</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D26" s="15" t="n">
         <v>19</v>
@@ -4009,10 +4069,10 @@
         <v>6</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I26" s="17" t="n">
         <v>0</v>
@@ -4036,10 +4096,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D27" s="15" t="n">
         <v>25</v>
@@ -4051,10 +4111,10 @@
         <v>7</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H27" s="16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I27" s="17" t="n">
         <v>0</v>
@@ -4078,10 +4138,10 @@
         <v>26</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D28" s="15" t="n">
         <v>12</v>
@@ -4093,10 +4153,10 @@
         <v>8</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I28" s="17" t="n">
         <v>0</v>
@@ -4120,10 +4180,10 @@
         <v>27</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D29" s="19" t="n">
         <v>9</v>
@@ -4135,10 +4195,10 @@
         <v>15</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H29" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I29" s="19"/>
       <c r="J29" s="19"/>
@@ -4157,10 +4217,10 @@
         <v>28</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D30" s="19" t="n">
         <v>1</v>
@@ -4172,10 +4232,10 @@
         <v>22</v>
       </c>
       <c r="G30" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H30" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I30" s="19"/>
       <c r="J30" s="19"/>
@@ -4194,10 +4254,10 @@
         <v>29</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D31" s="19" t="n">
         <v>6</v>
@@ -4209,10 +4269,10 @@
         <v>23</v>
       </c>
       <c r="G31" s="19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H31" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I31" s="19"/>
       <c r="J31" s="19"/>
@@ -4231,10 +4291,10 @@
         <v>30</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D32" s="19" t="n">
         <v>4</v>
@@ -4246,10 +4306,10 @@
         <v>30</v>
       </c>
       <c r="G32" s="19" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H32" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I32" s="19"/>
       <c r="J32" s="19"/>
@@ -4268,10 +4328,10 @@
         <v>31</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D33" s="19" t="n">
         <v>15</v>
@@ -4283,10 +4343,10 @@
         <v>47</v>
       </c>
       <c r="G33" s="19" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H33" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I33" s="19"/>
       <c r="J33" s="19"/>
@@ -4305,10 +4365,10 @@
         <v>32</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D34" s="19" t="n">
         <v>10</v>
@@ -4320,10 +4380,10 @@
         <v>5</v>
       </c>
       <c r="G34" s="19" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H34" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I34" s="19"/>
       <c r="J34" s="19"/>
@@ -4342,10 +4402,10 @@
         <v>33</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D35" s="19" t="n">
         <v>13</v>
@@ -4357,10 +4417,10 @@
         <v>9</v>
       </c>
       <c r="G35" s="19" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H35" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I35" s="19"/>
       <c r="J35" s="19"/>
@@ -4379,10 +4439,10 @@
         <v>34</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D36" s="19" t="n">
         <v>16</v>
@@ -4394,10 +4454,10 @@
         <v>19</v>
       </c>
       <c r="G36" s="19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H36" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I36" s="19"/>
       <c r="J36" s="19"/>
@@ -4416,10 +4476,10 @@
         <v>35</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D37" s="19" t="n">
         <v>4</v>
@@ -4431,10 +4491,10 @@
         <v>20</v>
       </c>
       <c r="G37" s="19" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H37" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I37" s="19"/>
       <c r="J37" s="19"/>
@@ -4453,10 +4513,10 @@
         <v>36</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D38" s="19" t="n">
         <v>4</v>
@@ -4468,10 +4528,10 @@
         <v>21</v>
       </c>
       <c r="G38" s="19" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H38" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I38" s="19"/>
       <c r="J38" s="19"/>
@@ -4490,10 +4550,10 @@
         <v>37</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D39" s="19" t="n">
         <v>14</v>
@@ -4505,10 +4565,10 @@
         <v>37</v>
       </c>
       <c r="G39" s="19" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H39" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I39" s="19"/>
       <c r="J39" s="19"/>
@@ -4527,10 +4587,10 @@
         <v>38</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D40" s="19" t="n">
         <v>7</v>
@@ -4542,10 +4602,10 @@
         <v>49</v>
       </c>
       <c r="G40" s="19" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H40" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I40" s="19"/>
       <c r="J40" s="19"/>
@@ -4564,10 +4624,10 @@
         <v>39</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D41" s="6" t="n">
         <v>11</v>
@@ -4579,7 +4639,7 @@
         <v>25</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H41" s="7" t="s">
         <v>21</v>
@@ -4616,10 +4676,10 @@
         <v>40</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D42" s="9" t="n">
         <v>2</v>
@@ -4631,7 +4691,7 @@
         <v>33</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H42" s="10" t="s">
         <v>21</v>
@@ -4668,10 +4728,10 @@
         <v>41</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D43" s="6" t="n">
         <v>32</v>
@@ -4683,7 +4743,7 @@
         <v>2</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H43" s="7" t="s">
         <v>21</v>
@@ -4720,10 +4780,10 @@
         <v>42</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D44" s="6" t="n">
         <v>39</v>
@@ -4735,7 +4795,7 @@
         <v>3</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H44" s="7" t="s">
         <v>21</v>
@@ -4772,10 +4832,10 @@
         <v>43</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D45" s="9" t="n">
         <v>3</v>
@@ -4787,7 +4847,7 @@
         <v>11</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H45" s="10" t="s">
         <v>21</v>
@@ -4824,10 +4884,10 @@
         <v>44</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D46" s="19" t="n">
         <v>1</v>
@@ -4839,10 +4899,10 @@
         <v>26</v>
       </c>
       <c r="G46" s="19" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H46" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I46" s="19"/>
       <c r="J46" s="19"/>
@@ -4858,10 +4918,10 @@
         <v>45</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D47" s="19" t="n">
         <v>9</v>
@@ -4873,10 +4933,10 @@
         <v>27</v>
       </c>
       <c r="G47" s="19" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H47" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I47" s="19"/>
       <c r="J47" s="19"/>
@@ -4892,10 +4952,10 @@
         <v>46</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D48" s="19" t="n">
         <v>8</v>
@@ -4907,10 +4967,10 @@
         <v>36</v>
       </c>
       <c r="G48" s="19" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H48" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I48" s="19"/>
       <c r="J48" s="19"/>
@@ -4926,10 +4986,10 @@
         <v>47</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D49" s="19" t="n">
         <v>3</v>
@@ -4941,10 +5001,10 @@
         <v>40</v>
       </c>
       <c r="G49" s="19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H49" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I49" s="19"/>
       <c r="J49" s="19"/>
@@ -4960,10 +5020,10 @@
         <v>48</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D50" s="19" t="n">
         <v>8</v>
@@ -4975,10 +5035,10 @@
         <v>48</v>
       </c>
       <c r="G50" s="19" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H50" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I50" s="19"/>
       <c r="J50" s="19"/>
@@ -4994,10 +5054,10 @@
         <v>49</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D51" s="19" t="n">
         <v>5</v>
@@ -5009,10 +5069,10 @@
         <v>10</v>
       </c>
       <c r="G51" s="19" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H51" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I51" s="19"/>
       <c r="J51" s="19"/>
@@ -5028,10 +5088,10 @@
         <v>50</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D52" s="19" t="n">
         <v>4</v>
@@ -5043,10 +5103,10 @@
         <v>13</v>
       </c>
       <c r="G52" s="19" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H52" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I52" s="19"/>
       <c r="J52" s="19"/>
@@ -5062,10 +5122,10 @@
         <v>51</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D53" s="19" t="n">
         <v>6</v>
@@ -5077,10 +5137,10 @@
         <v>14</v>
       </c>
       <c r="G53" s="19" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H53" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I53" s="19"/>
       <c r="J53" s="19"/>
@@ -5107,6 +5167,2258 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:N54"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="I3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="36.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="9" style="0" width="15.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="12.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="22" t="n">
+        <v>54</v>
+      </c>
+      <c r="E3" s="22" t="n">
+        <v>54</v>
+      </c>
+      <c r="F3" s="22" t="n">
+        <v>32</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="22" t="n">
+        <v>54</v>
+      </c>
+      <c r="J3" s="22" t="n">
+        <v>53</v>
+      </c>
+      <c r="K3" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" s="22" t="n">
+        <f aca="false">D3-I3</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="21" t="n">
+        <f aca="false">I3/D3</f>
+        <v>1</v>
+      </c>
+      <c r="N3" s="24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="22" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="22" t="n">
+        <v>13</v>
+      </c>
+      <c r="E4" s="22" t="n">
+        <v>13</v>
+      </c>
+      <c r="F4" s="22" t="n">
+        <v>44</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="22" t="n">
+        <f aca="false">J4+K4</f>
+        <v>13</v>
+      </c>
+      <c r="J4" s="22" t="n">
+        <v>13</v>
+      </c>
+      <c r="K4" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="22" t="n">
+        <f aca="false">D4-I4</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="21" t="n">
+        <f aca="false">I4/D4</f>
+        <v>1</v>
+      </c>
+      <c r="N4" s="24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="22" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="22" t="n">
+        <v>6</v>
+      </c>
+      <c r="E5" s="22" t="n">
+        <v>6</v>
+      </c>
+      <c r="F5" s="22" t="n">
+        <v>41</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="22" t="n">
+        <f aca="false">J5+K5</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="22" t="n">
+        <f aca="false">D5-I5</f>
+        <v>6</v>
+      </c>
+      <c r="M5" s="21" t="n">
+        <f aca="false">I5/D5</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="22" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="22" t="n">
+        <v>7</v>
+      </c>
+      <c r="E6" s="22" t="n">
+        <v>7</v>
+      </c>
+      <c r="F6" s="22" t="n">
+        <v>42</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="22" t="n">
+        <f aca="false">J6+K6</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="22" t="n">
+        <f aca="false">D6-I6</f>
+        <v>7</v>
+      </c>
+      <c r="M6" s="21" t="n">
+        <f aca="false">I6/D6</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="22" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="22" t="n">
+        <v>7</v>
+      </c>
+      <c r="E7" s="22" t="n">
+        <v>7</v>
+      </c>
+      <c r="F7" s="22" t="n">
+        <v>43</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="22" t="n">
+        <f aca="false">J7+K7</f>
+        <v>7</v>
+      </c>
+      <c r="J7" s="22" t="n">
+        <v>4</v>
+      </c>
+      <c r="K7" s="22" t="n">
+        <v>3</v>
+      </c>
+      <c r="L7" s="22" t="n">
+        <f aca="false">D7-I7</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="21" t="n">
+        <f aca="false">I7/D7</f>
+        <v>1</v>
+      </c>
+      <c r="N7" s="24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="22" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="22" t="n">
+        <v>17</v>
+      </c>
+      <c r="E8" s="22" t="n">
+        <v>17</v>
+      </c>
+      <c r="F8" s="22" t="n">
+        <v>24</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="22" t="n">
+        <f aca="false">J8+K8</f>
+        <v>13</v>
+      </c>
+      <c r="J8" s="22" t="n">
+        <v>12</v>
+      </c>
+      <c r="K8" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" s="22" t="n">
+        <f aca="false">D8-I8</f>
+        <v>4</v>
+      </c>
+      <c r="M8" s="21" t="n">
+        <f aca="false">I8/D8</f>
+        <v>0.764705882352941</v>
+      </c>
+      <c r="N8" s="24" t="n">
+        <v>0.705882352941176</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="22" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="22" t="n">
+        <v>16</v>
+      </c>
+      <c r="E9" s="22" t="n">
+        <v>16</v>
+      </c>
+      <c r="F9" s="22" t="n">
+        <v>28</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="22" t="n">
+        <f aca="false">J9+K9</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="22" t="n">
+        <f aca="false">D9-I9</f>
+        <v>16</v>
+      </c>
+      <c r="M9" s="21" t="n">
+        <f aca="false">I9/D9</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="22" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="22" t="n">
+        <v>18</v>
+      </c>
+      <c r="E10" s="22" t="n">
+        <v>18</v>
+      </c>
+      <c r="F10" s="22" t="n">
+        <v>29</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="22" t="n">
+        <f aca="false">J10+K10</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="22" t="n">
+        <f aca="false">D10-I10</f>
+        <v>18</v>
+      </c>
+      <c r="M10" s="21" t="n">
+        <f aca="false">I10/D10</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="22" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="22" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" s="22" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" s="22" t="n">
+        <v>38</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="22" t="n">
+        <f aca="false">J11+K11</f>
+        <v>2</v>
+      </c>
+      <c r="J11" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="22" t="n">
+        <v>2</v>
+      </c>
+      <c r="L11" s="22" t="n">
+        <f aca="false">D11-I11</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="21" t="n">
+        <f aca="false">I11/D11</f>
+        <v>1</v>
+      </c>
+      <c r="N11" s="24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="22" t="n">
+        <v>15</v>
+      </c>
+      <c r="E12" s="22" t="n">
+        <v>15</v>
+      </c>
+      <c r="F12" s="22" t="n">
+        <v>45</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="22" t="n">
+        <f aca="false">J12+K12</f>
+        <v>4</v>
+      </c>
+      <c r="J12" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" s="22" t="n">
+        <v>3</v>
+      </c>
+      <c r="L12" s="22" t="n">
+        <f aca="false">D12-I12</f>
+        <v>11</v>
+      </c>
+      <c r="M12" s="21" t="n">
+        <f aca="false">I12/D12</f>
+        <v>0.266666666666667</v>
+      </c>
+      <c r="N12" s="24" t="n">
+        <v>0.266666666666667</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="22" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="22" t="n">
+        <v>12</v>
+      </c>
+      <c r="E13" s="22" t="n">
+        <v>12</v>
+      </c>
+      <c r="F13" s="22" t="n">
+        <v>12</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="22" t="n">
+        <f aca="false">J13+K13</f>
+        <v>11</v>
+      </c>
+      <c r="J13" s="22" t="n">
+        <v>9</v>
+      </c>
+      <c r="K13" s="22" t="n">
+        <v>2</v>
+      </c>
+      <c r="L13" s="22" t="n">
+        <f aca="false">D13-I13</f>
+        <v>1</v>
+      </c>
+      <c r="M13" s="21" t="n">
+        <f aca="false">I13/D13</f>
+        <v>0.916666666666667</v>
+      </c>
+      <c r="N13" s="24" t="n">
+        <v>0.916666666666667</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="22" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="22" t="n">
+        <v>16</v>
+      </c>
+      <c r="E14" s="22" t="n">
+        <v>16</v>
+      </c>
+      <c r="F14" s="22" t="n">
+        <v>16</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="22" t="n">
+        <f aca="false">J14+K14</f>
+        <v>16</v>
+      </c>
+      <c r="J14" s="22" t="n">
+        <v>14</v>
+      </c>
+      <c r="K14" s="22" t="n">
+        <v>2</v>
+      </c>
+      <c r="L14" s="22" t="n">
+        <f aca="false">D14-I14</f>
+        <v>0</v>
+      </c>
+      <c r="M14" s="21" t="n">
+        <f aca="false">I14/D14</f>
+        <v>1</v>
+      </c>
+      <c r="N14" s="24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="22" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="22" t="n">
+        <v>14</v>
+      </c>
+      <c r="E15" s="22" t="n">
+        <v>14</v>
+      </c>
+      <c r="F15" s="22" t="n">
+        <v>17</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" s="22" t="n">
+        <f aca="false">J15+K15</f>
+        <v>9</v>
+      </c>
+      <c r="J15" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="22" t="n">
+        <v>9</v>
+      </c>
+      <c r="L15" s="22" t="n">
+        <f aca="false">D15-I15</f>
+        <v>5</v>
+      </c>
+      <c r="M15" s="21" t="n">
+        <f aca="false">I15/D15</f>
+        <v>0.642857142857143</v>
+      </c>
+      <c r="N15" s="24" t="n">
+        <v>0.642857142857143</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="22" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="22" t="n">
+        <v>15</v>
+      </c>
+      <c r="E16" s="22" t="n">
+        <v>15</v>
+      </c>
+      <c r="F16" s="22" t="n">
+        <v>18</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="22" t="n">
+        <f aca="false">J16+K16</f>
+        <v>5</v>
+      </c>
+      <c r="J16" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" s="22" t="n">
+        <v>4</v>
+      </c>
+      <c r="L16" s="22" t="n">
+        <f aca="false">D16-I16</f>
+        <v>10</v>
+      </c>
+      <c r="M16" s="21" t="n">
+        <f aca="false">I16/D16</f>
+        <v>0.333333333333333</v>
+      </c>
+      <c r="N16" s="24" t="n">
+        <v>0.333333333333333</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="22" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="22" t="n">
+        <v>17</v>
+      </c>
+      <c r="E17" s="22" t="n">
+        <v>17</v>
+      </c>
+      <c r="F17" s="22" t="n">
+        <v>31</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="22" t="n">
+        <f aca="false">J17+K17</f>
+        <v>16</v>
+      </c>
+      <c r="J17" s="22" t="n">
+        <v>16</v>
+      </c>
+      <c r="K17" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" s="22" t="n">
+        <f aca="false">D17-I17</f>
+        <v>1</v>
+      </c>
+      <c r="M17" s="21" t="n">
+        <f aca="false">I17/D17</f>
+        <v>0.941176470588235</v>
+      </c>
+      <c r="N17" s="24" t="n">
+        <v>0.941176470588235</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="22" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="22" t="n">
+        <v>2</v>
+      </c>
+      <c r="E18" s="22" t="n">
+        <v>2</v>
+      </c>
+      <c r="F18" s="22" t="n">
+        <v>35</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" s="22" t="n">
+        <f aca="false">J18+K18</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" s="22" t="n">
+        <f aca="false">D18-I18</f>
+        <v>2</v>
+      </c>
+      <c r="M18" s="21" t="n">
+        <f aca="false">I18/D18</f>
+        <v>0</v>
+      </c>
+      <c r="N18" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="22" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="22" t="n">
+        <v>16</v>
+      </c>
+      <c r="E19" s="22" t="n">
+        <v>16</v>
+      </c>
+      <c r="F19" s="22" t="n">
+        <v>46</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="22" t="n">
+        <f aca="false">J19+K19</f>
+        <v>8</v>
+      </c>
+      <c r="J19" s="22" t="n">
+        <v>6</v>
+      </c>
+      <c r="K19" s="22" t="n">
+        <v>2</v>
+      </c>
+      <c r="L19" s="22" t="n">
+        <f aca="false">D19-I19</f>
+        <v>8</v>
+      </c>
+      <c r="M19" s="21" t="n">
+        <f aca="false">I19/D19</f>
+        <v>0.5</v>
+      </c>
+      <c r="N19" s="24" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="22" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="22" t="n">
+        <v>18</v>
+      </c>
+      <c r="E20" s="22" t="n">
+        <v>18</v>
+      </c>
+      <c r="F20" s="22" t="n">
+        <v>50</v>
+      </c>
+      <c r="G20" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="22" t="n">
+        <f aca="false">J20+K20</f>
+        <v>14</v>
+      </c>
+      <c r="J20" s="22" t="n">
+        <v>5</v>
+      </c>
+      <c r="K20" s="22" t="n">
+        <v>9</v>
+      </c>
+      <c r="L20" s="22" t="n">
+        <f aca="false">D20-I20</f>
+        <v>4</v>
+      </c>
+      <c r="M20" s="21" t="n">
+        <f aca="false">I20/D20</f>
+        <v>0.777777777777778</v>
+      </c>
+      <c r="N20" s="24" t="n">
+        <v>0.722222222222222</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="22" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="22" t="n">
+        <v>2</v>
+      </c>
+      <c r="E21" s="22" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" s="22" t="n">
+        <v>4</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="H21" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="22" t="n">
+        <f aca="false">J21+K21</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" s="22" t="n">
+        <f aca="false">D21-I21</f>
+        <v>2</v>
+      </c>
+      <c r="M21" s="21" t="n">
+        <f aca="false">I21/D21</f>
+        <v>0</v>
+      </c>
+      <c r="N21" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="22" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="22" t="n">
+        <v>29</v>
+      </c>
+      <c r="E22" s="22" t="n">
+        <v>29</v>
+      </c>
+      <c r="F22" s="22" t="n">
+        <v>34</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="H22" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I22" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" s="25" t="n">
+        <f aca="false">D22-I22</f>
+        <v>29</v>
+      </c>
+      <c r="M22" s="21" t="n">
+        <f aca="false">I22/D22</f>
+        <v>0</v>
+      </c>
+      <c r="N22" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="22" t="n">
+        <v>19</v>
+      </c>
+      <c r="E23" s="22" t="n">
+        <v>19</v>
+      </c>
+      <c r="F23" s="22" t="n">
+        <v>39</v>
+      </c>
+      <c r="G23" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="H23" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I23" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" s="25" t="n">
+        <f aca="false">D23-I23</f>
+        <v>19</v>
+      </c>
+      <c r="M23" s="21" t="n">
+        <f aca="false">I23/D23</f>
+        <v>0</v>
+      </c>
+      <c r="N23" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="22" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="22" t="n">
+        <v>16</v>
+      </c>
+      <c r="E24" s="22" t="n">
+        <v>16</v>
+      </c>
+      <c r="F24" s="22" t="n">
+        <v>51</v>
+      </c>
+      <c r="G24" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="H24" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I24" s="25" t="n">
+        <v>14</v>
+      </c>
+      <c r="J24" s="25" t="n">
+        <v>14</v>
+      </c>
+      <c r="K24" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" s="25" t="n">
+        <f aca="false">D24-I24</f>
+        <v>2</v>
+      </c>
+      <c r="M24" s="21" t="n">
+        <f aca="false">I24/D24</f>
+        <v>0.875</v>
+      </c>
+      <c r="N24" s="24" t="n">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="22" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="22" t="n">
+        <v>17</v>
+      </c>
+      <c r="E25" s="22" t="n">
+        <v>17</v>
+      </c>
+      <c r="F25" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="H25" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I25" s="25" t="n">
+        <v>16</v>
+      </c>
+      <c r="J25" s="25" t="n">
+        <v>16</v>
+      </c>
+      <c r="K25" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" s="25" t="n">
+        <f aca="false">D25-I25</f>
+        <v>1</v>
+      </c>
+      <c r="M25" s="21" t="n">
+        <f aca="false">I25/D25</f>
+        <v>0.941176470588235</v>
+      </c>
+      <c r="N25" s="24" t="n">
+        <v>0.941176470588235</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="22" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="22" t="n">
+        <v>19</v>
+      </c>
+      <c r="E26" s="22" t="n">
+        <v>19</v>
+      </c>
+      <c r="F26" s="22" t="n">
+        <v>6</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="H26" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I26" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" s="25" t="n">
+        <f aca="false">D26-I26</f>
+        <v>19</v>
+      </c>
+      <c r="M26" s="21" t="n">
+        <f aca="false">I26/D26</f>
+        <v>0</v>
+      </c>
+      <c r="N26" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="22" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="22" t="n">
+        <v>25</v>
+      </c>
+      <c r="E27" s="22" t="n">
+        <v>25</v>
+      </c>
+      <c r="F27" s="22" t="n">
+        <v>7</v>
+      </c>
+      <c r="G27" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="H27" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I27" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" s="25" t="n">
+        <f aca="false">D27-I27</f>
+        <v>25</v>
+      </c>
+      <c r="M27" s="21" t="n">
+        <f aca="false">I27/D27</f>
+        <v>0</v>
+      </c>
+      <c r="N27" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="22" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="22" t="n">
+        <v>12</v>
+      </c>
+      <c r="E28" s="22" t="n">
+        <v>12</v>
+      </c>
+      <c r="F28" s="22" t="n">
+        <v>8</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="H28" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I28" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" s="25" t="n">
+        <f aca="false">D28-I28</f>
+        <v>12</v>
+      </c>
+      <c r="M28" s="21" t="n">
+        <f aca="false">I28/D28</f>
+        <v>0</v>
+      </c>
+      <c r="N28" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="22" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="22" t="n">
+        <v>9</v>
+      </c>
+      <c r="E29" s="22" t="n">
+        <v>9</v>
+      </c>
+      <c r="F29" s="22" t="n">
+        <v>15</v>
+      </c>
+      <c r="G29" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="H29" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="21" t="n">
+        <f aca="false">I29/D29</f>
+        <v>0</v>
+      </c>
+      <c r="N29" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="22" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="E30" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F30" s="22" t="n">
+        <v>22</v>
+      </c>
+      <c r="G30" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="H30" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="21" t="n">
+        <f aca="false">I30/D30</f>
+        <v>0</v>
+      </c>
+      <c r="N30" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="22" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" s="22" t="n">
+        <v>6</v>
+      </c>
+      <c r="E31" s="22" t="n">
+        <v>6</v>
+      </c>
+      <c r="F31" s="22" t="n">
+        <v>23</v>
+      </c>
+      <c r="G31" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="H31" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="22"/>
+      <c r="M31" s="21" t="n">
+        <f aca="false">I31/D31</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="22" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" s="22" t="n">
+        <v>4</v>
+      </c>
+      <c r="E32" s="22" t="n">
+        <v>4</v>
+      </c>
+      <c r="F32" s="22" t="n">
+        <v>30</v>
+      </c>
+      <c r="G32" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="H32" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="22"/>
+      <c r="M32" s="21" t="n">
+        <f aca="false">I32/D32</f>
+        <v>0</v>
+      </c>
+      <c r="N32" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="22" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" s="22" t="n">
+        <v>15</v>
+      </c>
+      <c r="E33" s="22" t="n">
+        <v>15</v>
+      </c>
+      <c r="F33" s="22" t="n">
+        <v>47</v>
+      </c>
+      <c r="G33" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="H33" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="21" t="n">
+        <f aca="false">I33/D33</f>
+        <v>0</v>
+      </c>
+      <c r="N33" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="22" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="D34" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="E34" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="F34" s="22" t="n">
+        <v>5</v>
+      </c>
+      <c r="G34" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="H34" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="22"/>
+      <c r="M34" s="21" t="n">
+        <f aca="false">I34/D34</f>
+        <v>0</v>
+      </c>
+      <c r="N34" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="22" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="22" t="n">
+        <v>13</v>
+      </c>
+      <c r="E35" s="22" t="n">
+        <v>13</v>
+      </c>
+      <c r="F35" s="22" t="n">
+        <v>9</v>
+      </c>
+      <c r="G35" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="H35" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="21" t="n">
+        <f aca="false">I35/D35</f>
+        <v>0</v>
+      </c>
+      <c r="N35" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="22" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" s="22" t="n">
+        <v>16</v>
+      </c>
+      <c r="E36" s="22" t="n">
+        <v>16</v>
+      </c>
+      <c r="F36" s="22" t="n">
+        <v>19</v>
+      </c>
+      <c r="G36" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="H36" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I36" s="22"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="21" t="n">
+        <f aca="false">I36/D36</f>
+        <v>0</v>
+      </c>
+      <c r="N36" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="22" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="D37" s="22" t="n">
+        <v>4</v>
+      </c>
+      <c r="E37" s="22" t="n">
+        <v>4</v>
+      </c>
+      <c r="F37" s="22" t="n">
+        <v>20</v>
+      </c>
+      <c r="G37" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="H37" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I37" s="22"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
+      <c r="L37" s="22"/>
+      <c r="M37" s="21" t="n">
+        <f aca="false">I37/D37</f>
+        <v>0</v>
+      </c>
+      <c r="N37" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="22" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38" s="22" t="n">
+        <v>4</v>
+      </c>
+      <c r="E38" s="22" t="n">
+        <v>4</v>
+      </c>
+      <c r="F38" s="22" t="n">
+        <v>21</v>
+      </c>
+      <c r="G38" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="H38" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
+      <c r="K38" s="22"/>
+      <c r="L38" s="22"/>
+      <c r="M38" s="21" t="n">
+        <f aca="false">I38/D38</f>
+        <v>0</v>
+      </c>
+      <c r="N38" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="22" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="D39" s="22" t="n">
+        <v>14</v>
+      </c>
+      <c r="E39" s="22" t="n">
+        <v>14</v>
+      </c>
+      <c r="F39" s="22" t="n">
+        <v>37</v>
+      </c>
+      <c r="G39" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="H39" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I39" s="22"/>
+      <c r="J39" s="22"/>
+      <c r="K39" s="22"/>
+      <c r="L39" s="22"/>
+      <c r="M39" s="21" t="n">
+        <f aca="false">I39/D39</f>
+        <v>0</v>
+      </c>
+      <c r="N39" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="22" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="D40" s="22" t="n">
+        <v>7</v>
+      </c>
+      <c r="E40" s="22" t="n">
+        <v>7</v>
+      </c>
+      <c r="F40" s="22" t="n">
+        <v>49</v>
+      </c>
+      <c r="G40" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="H40" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I40" s="22"/>
+      <c r="J40" s="22"/>
+      <c r="K40" s="22"/>
+      <c r="L40" s="22"/>
+      <c r="M40" s="21" t="n">
+        <f aca="false">I40/D40</f>
+        <v>0</v>
+      </c>
+      <c r="N40" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="22" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C41" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="D41" s="22" t="n">
+        <v>11</v>
+      </c>
+      <c r="E41" s="22" t="n">
+        <v>11</v>
+      </c>
+      <c r="F41" s="22" t="n">
+        <v>25</v>
+      </c>
+      <c r="G41" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="H41" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I41" s="22" t="n">
+        <f aca="false">J41+K41</f>
+        <v>11</v>
+      </c>
+      <c r="J41" s="22" t="n">
+        <v>11</v>
+      </c>
+      <c r="K41" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L41" s="22" t="n">
+        <f aca="false">D41-I41</f>
+        <v>0</v>
+      </c>
+      <c r="M41" s="21" t="n">
+        <f aca="false">I41/D41</f>
+        <v>1</v>
+      </c>
+      <c r="N41" s="24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="22" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42" s="22" t="n">
+        <v>2</v>
+      </c>
+      <c r="E42" s="22" t="n">
+        <v>2</v>
+      </c>
+      <c r="F42" s="22" t="n">
+        <v>33</v>
+      </c>
+      <c r="G42" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="H42" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I42" s="22" t="n">
+        <f aca="false">J42+K42</f>
+        <v>0</v>
+      </c>
+      <c r="J42" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" s="22" t="n">
+        <f aca="false">D42-I42</f>
+        <v>2</v>
+      </c>
+      <c r="M42" s="21" t="n">
+        <f aca="false">I42/D42</f>
+        <v>0</v>
+      </c>
+      <c r="N42" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="22" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="D43" s="22" t="n">
+        <v>32</v>
+      </c>
+      <c r="E43" s="22" t="n">
+        <v>32</v>
+      </c>
+      <c r="F43" s="22" t="n">
+        <v>2</v>
+      </c>
+      <c r="G43" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="H43" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I43" s="22" t="n">
+        <f aca="false">J43+K43</f>
+        <v>32</v>
+      </c>
+      <c r="J43" s="22" t="n">
+        <v>32</v>
+      </c>
+      <c r="K43" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L43" s="22" t="n">
+        <f aca="false">D43-I43</f>
+        <v>0</v>
+      </c>
+      <c r="M43" s="21" t="n">
+        <f aca="false">I43/D43</f>
+        <v>1</v>
+      </c>
+      <c r="N43" s="24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="22" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="D44" s="22" t="n">
+        <v>39</v>
+      </c>
+      <c r="E44" s="22" t="n">
+        <v>39</v>
+      </c>
+      <c r="F44" s="22" t="n">
+        <v>3</v>
+      </c>
+      <c r="G44" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="H44" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I44" s="22" t="n">
+        <f aca="false">J44+K44</f>
+        <v>38</v>
+      </c>
+      <c r="J44" s="22" t="n">
+        <v>35</v>
+      </c>
+      <c r="K44" s="22" t="n">
+        <v>3</v>
+      </c>
+      <c r="L44" s="22" t="n">
+        <f aca="false">D44-I44</f>
+        <v>1</v>
+      </c>
+      <c r="M44" s="21" t="n">
+        <f aca="false">I44/D44</f>
+        <v>0.974358974358974</v>
+      </c>
+      <c r="N44" s="24" t="n">
+        <v>0.974358974358974</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="22" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="C45" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="D45" s="22" t="n">
+        <v>3</v>
+      </c>
+      <c r="E45" s="22" t="n">
+        <v>3</v>
+      </c>
+      <c r="F45" s="22" t="n">
+        <v>11</v>
+      </c>
+      <c r="G45" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="H45" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I45" s="22" t="n">
+        <f aca="false">J45+K45</f>
+        <v>0</v>
+      </c>
+      <c r="J45" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K45" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L45" s="22" t="n">
+        <f aca="false">D45-I45</f>
+        <v>3</v>
+      </c>
+      <c r="M45" s="21" t="n">
+        <f aca="false">I45/D45</f>
+        <v>0</v>
+      </c>
+      <c r="N45" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="22" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="C46" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D46" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="E46" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F46" s="22" t="n">
+        <v>26</v>
+      </c>
+      <c r="G46" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H46" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
+      <c r="K46" s="22"/>
+      <c r="L46" s="22"/>
+      <c r="M46" s="22"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="22" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C47" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D47" s="22" t="n">
+        <v>9</v>
+      </c>
+      <c r="E47" s="22" t="n">
+        <v>9</v>
+      </c>
+      <c r="F47" s="22" t="n">
+        <v>27</v>
+      </c>
+      <c r="G47" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="H47" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
+      <c r="K47" s="22"/>
+      <c r="L47" s="22"/>
+      <c r="M47" s="22"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="22" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D48" s="22" t="n">
+        <v>8</v>
+      </c>
+      <c r="E48" s="22" t="n">
+        <v>8</v>
+      </c>
+      <c r="F48" s="22" t="n">
+        <v>36</v>
+      </c>
+      <c r="G48" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="H48" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I48" s="22"/>
+      <c r="J48" s="22"/>
+      <c r="K48" s="22"/>
+      <c r="L48" s="22"/>
+      <c r="M48" s="22"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="22" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="C49" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D49" s="22" t="n">
+        <v>3</v>
+      </c>
+      <c r="E49" s="22" t="n">
+        <v>3</v>
+      </c>
+      <c r="F49" s="22" t="n">
+        <v>40</v>
+      </c>
+      <c r="G49" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="H49" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I49" s="22"/>
+      <c r="J49" s="22"/>
+      <c r="K49" s="22"/>
+      <c r="L49" s="22"/>
+      <c r="M49" s="22"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="22" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D50" s="22" t="n">
+        <v>8</v>
+      </c>
+      <c r="E50" s="22" t="n">
+        <v>8</v>
+      </c>
+      <c r="F50" s="22" t="n">
+        <v>48</v>
+      </c>
+      <c r="G50" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="H50" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I50" s="22"/>
+      <c r="J50" s="22"/>
+      <c r="K50" s="22"/>
+      <c r="L50" s="22"/>
+      <c r="M50" s="22"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="22" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="C51" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D51" s="22" t="n">
+        <v>5</v>
+      </c>
+      <c r="E51" s="22" t="n">
+        <v>5</v>
+      </c>
+      <c r="F51" s="22" t="n">
+        <v>10</v>
+      </c>
+      <c r="G51" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="H51" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I51" s="22"/>
+      <c r="J51" s="22"/>
+      <c r="K51" s="22"/>
+      <c r="L51" s="22"/>
+      <c r="M51" s="22"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="22" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D52" s="22" t="n">
+        <v>4</v>
+      </c>
+      <c r="E52" s="22" t="n">
+        <v>4</v>
+      </c>
+      <c r="F52" s="22" t="n">
+        <v>13</v>
+      </c>
+      <c r="G52" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="H52" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I52" s="22"/>
+      <c r="J52" s="22"/>
+      <c r="K52" s="22"/>
+      <c r="L52" s="22"/>
+      <c r="M52" s="22"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="22" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="C53" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D53" s="22" t="n">
+        <v>6</v>
+      </c>
+      <c r="E53" s="22" t="n">
+        <v>6</v>
+      </c>
+      <c r="F53" s="22" t="n">
+        <v>14</v>
+      </c>
+      <c r="G53" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="H53" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I53" s="22"/>
+      <c r="J53" s="22"/>
+      <c r="K53" s="22"/>
+      <c r="L53" s="22"/>
+      <c r="M53" s="22"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="26"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="26"/>
+      <c r="H54" s="26"/>
+      <c r="I54" s="26"/>
+      <c r="J54" s="26"/>
+      <c r="K54" s="26"/>
+      <c r="L54" s="26"/>
+      <c r="M54" s="26"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I1:L1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Arial,標準"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Arial,標準"ページ &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -5130,65 +7442,65 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="22" t="n">
+      <c r="C2" s="24" t="n">
         <f aca="false">SUM(結果まとめ!J3:J4)/SUM(結果まとめ!D3:D4)</f>
         <v>0.985074626865672</v>
       </c>
-      <c r="D2" s="22" t="n">
+      <c r="D2" s="24" t="n">
         <f aca="false">SUM(結果まとめ!I3:I4)/SUM(結果まとめ!D3:D4)</f>
         <v>1</v>
       </c>
-      <c r="E2" s="22" t="n">
+      <c r="E2" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="22" t="n">
+      <c r="F2" s="24" t="n">
         <v>0.97</v>
       </c>
-      <c r="G2" s="22" t="n">
+      <c r="G2" s="24" t="n">
         <v>0.97</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="C3" s="22" t="n">
+        <v>117</v>
+      </c>
+      <c r="C3" s="24" t="n">
         <f aca="false">SUM(結果まとめ!J41:J45)/SUM(結果まとめ!D41:D45)</f>
         <v>0.896551724137931</v>
       </c>
-      <c r="D3" s="22" t="n">
+      <c r="D3" s="24" t="n">
         <f aca="false">SUM(結果まとめ!I41:I45)/SUM(結果まとめ!D41:D45)</f>
         <v>0.931034482758621</v>
       </c>
-      <c r="E3" s="22" t="n">
+      <c r="E3" s="24" t="n">
         <v>0.89</v>
       </c>
-      <c r="F3" s="22" t="n">
+      <c r="F3" s="24" t="n">
         <v>0.92</v>
       </c>
-      <c r="G3" s="22" t="n">
+      <c r="G3" s="24" t="n">
         <v>0.9</v>
       </c>
     </row>
@@ -5196,21 +7508,21 @@
       <c r="B4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="22" t="n">
+      <c r="C4" s="24" t="n">
         <f aca="false">SUM(結果まとめ!J5:J7)/SUM(結果まとめ!D5:D7)</f>
         <v>0.2</v>
       </c>
-      <c r="D4" s="22" t="n">
+      <c r="D4" s="24" t="n">
         <f aca="false">SUM(結果まとめ!I5:I7)/SUM(結果まとめ!D5:D7)</f>
         <v>0.35</v>
       </c>
-      <c r="E4" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="22" t="n">
+      <c r="E4" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="24" t="n">
         <v>0.6</v>
       </c>
-      <c r="G4" s="22" t="n">
+      <c r="G4" s="24" t="n">
         <v>0.15</v>
       </c>
     </row>
@@ -5218,43 +7530,43 @@
       <c r="B5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="22" t="n">
+      <c r="C5" s="24" t="n">
         <f aca="false">SUM(結果まとめ!J8:J14)/SUM(結果まとめ!D8:D14)</f>
         <v>0.385416666666667</v>
       </c>
-      <c r="D5" s="22" t="n">
+      <c r="D5" s="24" t="n">
         <f aca="false">SUM(結果まとめ!I8:I14)/SUM(結果まとめ!D8:D14)</f>
-        <v>0.53125</v>
-      </c>
-      <c r="E5" s="22" t="n">
+        <v>0.46875</v>
+      </c>
+      <c r="E5" s="24" t="n">
         <v>0.61</v>
       </c>
-      <c r="F5" s="22" t="n">
+      <c r="F5" s="24" t="n">
         <v>0.2</v>
       </c>
-      <c r="G5" s="22" t="n">
+      <c r="G5" s="24" t="n">
         <v>0.55</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="22" t="n">
+        <v>54</v>
+      </c>
+      <c r="C6" s="24" t="n">
         <f aca="false">SUM(結果まとめ!J15:J21)/SUM(結果まとめ!D15:D21)</f>
         <v>0.321428571428571</v>
       </c>
-      <c r="D6" s="22" t="n">
+      <c r="D6" s="24" t="n">
         <f aca="false">SUM(結果まとめ!I15:I21)/SUM(結果まとめ!D15:D21)</f>
         <v>0.607142857142857</v>
       </c>
-      <c r="E6" s="22" t="n">
+      <c r="E6" s="24" t="n">
         <v>0.52</v>
       </c>
-      <c r="F6" s="22" t="n">
+      <c r="F6" s="24" t="n">
         <v>0.69</v>
       </c>
-      <c r="G6" s="22" t="n">
+      <c r="G6" s="24" t="n">
         <v>0.69</v>
       </c>
     </row>
@@ -5270,7 +7582,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -5293,54 +7605,54 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="22" t="n">
+      <c r="C2" s="24" t="n">
         <f aca="false">1-SUM(結果まとめ!N3:N4)/SUM(結果まとめ!E3:E4)</f>
         <v>1</v>
       </c>
-      <c r="D2" s="22" t="n">
+      <c r="D2" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="22" t="n">
+      <c r="E2" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="22" t="n">
+      <c r="F2" s="24" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="C3" s="22" t="n">
+        <v>117</v>
+      </c>
+      <c r="C3" s="24" t="n">
         <f aca="false">1-SUM(結果まとめ!N41:N45)/SUM(結果まとめ!E41:E45)</f>
         <v>0.954022988505747</v>
       </c>
-      <c r="D3" s="22" t="n">
+      <c r="D3" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="22" t="n">
+      <c r="E3" s="24" t="n">
         <v>0.95</v>
       </c>
-      <c r="F3" s="22" t="n">
+      <c r="F3" s="24" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5348,17 +7660,17 @@
       <c r="B4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="22" t="n">
+      <c r="C4" s="24" t="n">
         <f aca="false">1-SUM(結果まとめ!N5:N7)/SUM(結果まとめ!E5:E7)</f>
         <v>0.85</v>
       </c>
-      <c r="D4" s="22" t="n">
+      <c r="D4" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="22" t="n">
+      <c r="E4" s="24" t="n">
         <v>0.7</v>
       </c>
-      <c r="F4" s="22" t="n">
+      <c r="F4" s="24" t="n">
         <v>0.85</v>
       </c>
     </row>
@@ -5366,41 +7678,41 @@
       <c r="B5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="22" t="n">
+      <c r="C5" s="24" t="n">
         <f aca="false">1-SUM(結果まとめ!N8:N14)/SUM(結果まとめ!E8:E14)</f>
         <v>1</v>
       </c>
-      <c r="D5" s="22" t="n">
+      <c r="D5" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="E5" s="22" t="n">
+      <c r="E5" s="24" t="n">
         <v>0.9</v>
       </c>
-      <c r="F5" s="22" t="n">
+      <c r="F5" s="24" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="22" t="n">
+        <v>54</v>
+      </c>
+      <c r="C6" s="24" t="n">
         <f aca="false">1-SUM(結果まとめ!N15:N21)/SUM(結果まとめ!E15:E21)</f>
         <v>0.964285714285714</v>
       </c>
-      <c r="D6" s="22" t="n">
+      <c r="D6" s="24" t="n">
         <v>0.96</v>
       </c>
-      <c r="E6" s="22" t="n">
+      <c r="E6" s="24" t="n">
         <v>0.93</v>
       </c>
-      <c r="F6" s="22" t="n">
+      <c r="F6" s="24" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F7" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -5415,7 +7727,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -5441,13 +7753,13 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5455,13 +7767,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5469,13 +7781,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5483,13 +7795,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5497,13 +7809,13 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5511,13 +7823,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5525,13 +7837,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5539,13 +7851,13 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5553,13 +7865,13 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5567,13 +7879,13 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5581,13 +7893,13 @@
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5595,13 +7907,13 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5609,13 +7921,13 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5623,13 +7935,13 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5637,13 +7949,13 @@
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5651,13 +7963,13 @@
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5665,13 +7977,13 @@
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5679,13 +7991,13 @@
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5693,13 +8005,13 @@
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5707,13 +8019,13 @@
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5721,13 +8033,13 @@
         <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5735,13 +8047,13 @@
         <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5749,13 +8061,13 @@
         <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5763,13 +8075,13 @@
         <v>23</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5777,13 +8089,13 @@
         <v>24</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5791,13 +8103,13 @@
         <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5805,13 +8117,13 @@
         <v>26</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5819,13 +8131,13 @@
         <v>27</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5833,13 +8145,13 @@
         <v>28</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5847,13 +8159,13 @@
         <v>29</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5861,13 +8173,13 @@
         <v>30</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5875,13 +8187,13 @@
         <v>31</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5889,13 +8201,13 @@
         <v>32</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5903,13 +8215,13 @@
         <v>33</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5917,13 +8229,13 @@
         <v>34</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5931,13 +8243,13 @@
         <v>35</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5945,13 +8257,13 @@
         <v>36</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5959,13 +8271,13 @@
         <v>37</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5973,13 +8285,13 @@
         <v>38</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5987,13 +8299,13 @@
         <v>39</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6001,13 +8313,13 @@
         <v>40</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6015,13 +8327,13 @@
         <v>41</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6029,13 +8341,13 @@
         <v>42</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>241</v>
-      </c>
       <c r="E43" s="1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6043,13 +8355,13 @@
         <v>43</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6057,13 +8369,13 @@
         <v>44</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6071,13 +8383,13 @@
         <v>45</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6085,13 +8397,13 @@
         <v>46</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6099,13 +8411,13 @@
         <v>47</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6113,13 +8425,13 @@
         <v>48</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6127,13 +8439,13 @@
         <v>49</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6141,13 +8453,13 @@
         <v>50</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6155,13 +8467,13 @@
         <v>51</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>